<commit_message>
Updated for tfs 6145.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C37040
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3165" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3170" uniqueCount="832">
   <si>
     <t>SourceID</t>
   </si>
@@ -2531,6 +2531,18 @@
   </si>
   <si>
     <t>Added NPN Description tab</t>
+  </si>
+  <si>
+    <t>updated DIM_Coaching_Reason andDIM_SubCoaching_Reason tabs to add values for Breaks feeds</t>
+  </si>
+  <si>
+    <t>Breaks</t>
+  </si>
+  <si>
+    <t>Exceed Number of Breaks</t>
+  </si>
+  <si>
+    <t>Exceed Break Length</t>
   </si>
 </sst>
 </file>
@@ -2895,9 +2907,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3770,6 +3784,23 @@
       </c>
       <c r="E51" t="s">
         <v>827</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>47</v>
+      </c>
+      <c r="B52" s="1">
+        <v>42838</v>
+      </c>
+      <c r="C52" t="s">
+        <v>432</v>
+      </c>
+      <c r="D52">
+        <v>6145</v>
+      </c>
+      <c r="E52" t="s">
+        <v>828</v>
       </c>
     </row>
   </sheetData>
@@ -30787,11 +30818,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
-    </sheetView>
+    <sheetView topLeftCell="A30" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -31255,6 +31284,14 @@
         <v>814</v>
       </c>
     </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>829</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31262,9 +31299,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B239"/>
+  <dimension ref="A1:B241"/>
   <sheetViews>
-    <sheetView topLeftCell="A195" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -33182,6 +33219,22 @@
       </c>
       <c r="B239" t="s">
         <v>809</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>238</v>
+      </c>
+      <c r="B240" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>239</v>
+      </c>
+      <c r="B241" t="s">
+        <v>831</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for parent TFS 8597- Changes to DTT feed load.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C38824
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3299" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3310" uniqueCount="891">
   <si>
     <t>SourceID</t>
   </si>
@@ -2716,6 +2716,9 @@
   </si>
   <si>
     <t>The timecard date and number of changes with incorrect change categories is shown below:</t>
+  </si>
+  <si>
+    <t>Updated Email_Notifications to support Pending Employee Review Generic DTT Feed</t>
   </si>
 </sst>
 </file>
@@ -3087,10 +3090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4082,6 +4085,23 @@
       </c>
       <c r="E59" t="s">
         <v>827</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>53</v>
+      </c>
+      <c r="B60" s="1">
+        <v>43020</v>
+      </c>
+      <c r="C60" t="s">
+        <v>432</v>
+      </c>
+      <c r="D60">
+        <v>8597</v>
+      </c>
+      <c r="E60" t="s">
+        <v>890</v>
       </c>
     </row>
   </sheetData>
@@ -20951,11 +20971,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K167"/>
+  <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166:I167"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -26748,31 +26766,31 @@
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A166" s="5" t="s">
+      <c r="A166" t="s">
         <v>175</v>
       </c>
-      <c r="B166" s="5" t="s">
+      <c r="B166" t="s">
         <v>832</v>
       </c>
-      <c r="C166" s="5" t="s">
+      <c r="C166" t="s">
         <v>3</v>
       </c>
-      <c r="D166" s="5" t="s">
+      <c r="D166" t="s">
         <v>828</v>
       </c>
-      <c r="E166" s="5">
-        <v>0</v>
-      </c>
-      <c r="F166" s="5" t="s">
+      <c r="E166">
+        <v>0</v>
+      </c>
+      <c r="F166" t="s">
         <v>26</v>
       </c>
-      <c r="G166" s="5" t="s">
+      <c r="G166" t="s">
         <v>425</v>
       </c>
-      <c r="H166" s="5" t="s">
+      <c r="H166" t="s">
         <v>386</v>
       </c>
-      <c r="I166" s="5" t="s">
+      <c r="I166" t="s">
         <v>473</v>
       </c>
       <c r="J166">
@@ -26783,37 +26801,72 @@
       </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A167" s="5" t="s">
+      <c r="A167" t="s">
         <v>92</v>
       </c>
-      <c r="B167" s="5" t="s">
+      <c r="B167" t="s">
         <v>15</v>
       </c>
-      <c r="C167" s="5" t="s">
+      <c r="C167" t="s">
         <v>3</v>
       </c>
-      <c r="D167" s="5" t="s">
+      <c r="D167" t="s">
         <v>470</v>
       </c>
-      <c r="E167" s="5">
-        <v>0</v>
-      </c>
-      <c r="F167" s="5" t="s">
+      <c r="E167">
+        <v>0</v>
+      </c>
+      <c r="F167" t="s">
         <v>26</v>
       </c>
-      <c r="G167" s="5" t="s">
+      <c r="G167" t="s">
         <v>425</v>
       </c>
-      <c r="H167" s="5" t="s">
+      <c r="H167" t="s">
         <v>386</v>
       </c>
-      <c r="I167" s="5" t="s">
+      <c r="I167" t="s">
         <v>833</v>
       </c>
       <c r="J167">
         <v>1</v>
       </c>
       <c r="K167" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A168" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>832</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>828</v>
+      </c>
+      <c r="E168" s="5">
+        <v>0</v>
+      </c>
+      <c r="F168" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G168" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="H168" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="I168" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="J168">
+        <v>1</v>
+      </c>
+      <c r="K168" t="s">
         <v>175</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Additional update for TFS 8587 from V&V feedback.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C38831
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3310" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3312" uniqueCount="892">
   <si>
     <t>SourceID</t>
   </si>
@@ -2719,6 +2719,9 @@
   </si>
   <si>
     <t>Updated Email_Notifications to support Pending Employee Review Generic DTT Feed</t>
+  </si>
+  <si>
+    <t>Updated Email_Notifications to support Pending Employee Review Generic DTT Feed (fixed incorrect Subject value from doc review feeedback)</t>
   </si>
 </sst>
 </file>
@@ -3090,10 +3093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4102,6 +4105,23 @@
       </c>
       <c r="E60" t="s">
         <v>890</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>53.1</v>
+      </c>
+      <c r="B61" s="1">
+        <v>43021</v>
+      </c>
+      <c r="C61" t="s">
+        <v>432</v>
+      </c>
+      <c r="D61">
+        <v>8597</v>
+      </c>
+      <c r="E61" t="s">
+        <v>891</v>
       </c>
     </row>
   </sheetData>
@@ -20973,7 +20993,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -26858,7 +26880,7 @@
         <v>425</v>
       </c>
       <c r="H168" s="5" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I168" s="5" t="s">
         <v>473</v>

</xml_diff>

<commit_message>
TFS 8793 - Additional modules to support Breaks feeds for non-exempt staff
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C39025
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3312" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3372" uniqueCount="897">
   <si>
     <t>SourceID</t>
   </si>
@@ -2722,6 +2722,21 @@
   </si>
   <si>
     <t>Updated Email_Notifications to support Pending Employee Review Generic DTT Feed (fixed incorrect Subject value from doc review feeedback)</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>Analytics Reporting</t>
+  </si>
+  <si>
+    <t>Production Planning</t>
+  </si>
+  <si>
+    <t>Program Analyst</t>
+  </si>
+  <si>
+    <t>Additional Modules to support BRL and BRN feeds. Upadted DIM_Module and Email_Notifications tabs</t>
   </si>
 </sst>
 </file>
@@ -3093,10 +3108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4122,6 +4137,23 @@
       </c>
       <c r="E61" t="s">
         <v>891</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>54</v>
+      </c>
+      <c r="B62" s="1">
+        <v>43056</v>
+      </c>
+      <c r="C62" t="s">
+        <v>432</v>
+      </c>
+      <c r="D62">
+        <v>8793</v>
+      </c>
+      <c r="E62" t="s">
+        <v>896</v>
       </c>
     </row>
   </sheetData>
@@ -20991,10 +21023,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K168"/>
+  <dimension ref="A1:K174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+    <sheetView topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="A169" sqref="A169:XFD174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26858,31 +26890,31 @@
       </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A168" s="5" t="s">
+      <c r="A168" t="s">
         <v>175</v>
       </c>
-      <c r="B168" s="5" t="s">
+      <c r="B168" t="s">
         <v>832</v>
       </c>
-      <c r="C168" s="5" t="s">
+      <c r="C168" t="s">
         <v>3</v>
       </c>
-      <c r="D168" s="5" t="s">
+      <c r="D168" t="s">
         <v>828</v>
       </c>
-      <c r="E168" s="5">
-        <v>0</v>
-      </c>
-      <c r="F168" s="5" t="s">
+      <c r="E168">
+        <v>0</v>
+      </c>
+      <c r="F168" t="s">
         <v>177</v>
       </c>
-      <c r="G168" s="5" t="s">
+      <c r="G168" t="s">
         <v>425</v>
       </c>
-      <c r="H168" s="5" t="s">
+      <c r="H168" t="s">
         <v>383</v>
       </c>
-      <c r="I168" s="5" t="s">
+      <c r="I168" t="s">
         <v>473</v>
       </c>
       <c r="J168">
@@ -26890,6 +26922,216 @@
       </c>
       <c r="K168" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="B169" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C169" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D169" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E169" s="5">
+        <v>0</v>
+      </c>
+      <c r="F169" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G169" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H169" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="I169" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="J169" s="5">
+        <v>0</v>
+      </c>
+      <c r="K169" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D170" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E170" s="5">
+        <v>0</v>
+      </c>
+      <c r="F170" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G170" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H170" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="I170" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="J170" s="5">
+        <v>0</v>
+      </c>
+      <c r="K170" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="5" t="s">
+        <v>894</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D171" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E171" s="5">
+        <v>0</v>
+      </c>
+      <c r="F171" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G171" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H171" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="I171" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="J171" s="5">
+        <v>0</v>
+      </c>
+      <c r="K171" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C172" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D172" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E172" s="5">
+        <v>0</v>
+      </c>
+      <c r="F172" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G172" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H172" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="I172" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="J172" s="5">
+        <v>0</v>
+      </c>
+      <c r="K172" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="B173" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C173" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D173" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E173" s="5">
+        <v>0</v>
+      </c>
+      <c r="F173" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G173" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H173" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="I173" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="J173" s="5">
+        <v>0</v>
+      </c>
+      <c r="K173" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C174" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D174" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E174" s="5">
+        <v>0</v>
+      </c>
+      <c r="F174" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G174" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H174" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="I174" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="J174" s="5">
+        <v>0</v>
+      </c>
+      <c r="K174" s="5" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -34361,9 +34603,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -34505,6 +34749,86 @@
       </c>
       <c r="F7">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>894</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 9091 - Additional sub Coaching Reason for CSR and Sup Modules
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C39057
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3372" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3377" uniqueCount="899">
   <si>
     <t>SourceID</t>
   </si>
@@ -2737,6 +2737,12 @@
   </si>
   <si>
     <t>Additional Modules to support BRL and BRN feeds. Upadted DIM_Module and Email_Notifications tabs</t>
+  </si>
+  <si>
+    <t>Attendance Improvement Discussion</t>
+  </si>
+  <si>
+    <t>New sub-coaching reason to Attendance for CSR and Supervisor. Updated Dim SubCoaching Reason and Coaching Reason Selection tabs.</t>
   </si>
 </sst>
 </file>
@@ -3108,10 +3114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4154,6 +4160,23 @@
       </c>
       <c r="E62" t="s">
         <v>896</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>55</v>
+      </c>
+      <c r="B63" s="1">
+        <v>43067</v>
+      </c>
+      <c r="C63" t="s">
+        <v>432</v>
+      </c>
+      <c r="D63">
+        <v>9091</v>
+      </c>
+      <c r="E63" t="s">
+        <v>898</v>
       </c>
     </row>
   </sheetData>
@@ -5579,9 +5602,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P306"/>
+  <dimension ref="A1:P307"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A282" workbookViewId="0">
+      <selection activeCell="A307" sqref="A307:P307"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -20886,6 +20911,56 @@
       </c>
       <c r="P306">
         <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A307" s="5">
+        <v>3</v>
+      </c>
+      <c r="B307" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C307" s="5">
+        <v>243</v>
+      </c>
+      <c r="D307" s="5" t="s">
+        <v>897</v>
+      </c>
+      <c r="E307" s="5">
+        <v>1</v>
+      </c>
+      <c r="F307" s="5">
+        <v>1</v>
+      </c>
+      <c r="G307" s="5">
+        <v>1</v>
+      </c>
+      <c r="H307" s="5">
+        <v>1</v>
+      </c>
+      <c r="I307" s="5">
+        <v>1</v>
+      </c>
+      <c r="J307" s="5">
+        <v>1</v>
+      </c>
+      <c r="K307" s="5">
+        <v>0</v>
+      </c>
+      <c r="L307" s="5">
+        <v>1</v>
+      </c>
+      <c r="M307" s="5">
+        <v>0</v>
+      </c>
+      <c r="N307" s="5">
+        <v>0</v>
+      </c>
+      <c r="O307" s="5">
+        <v>0</v>
+      </c>
+      <c r="P307" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -32086,10 +32161,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B244"/>
+  <dimension ref="A1:B245"/>
   <sheetViews>
-    <sheetView topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="A242" sqref="A242:B244"/>
+    <sheetView topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="B245" sqref="A245:B245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34027,27 +34102,35 @@
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A242" s="5">
+      <c r="A242">
         <v>240</v>
       </c>
-      <c r="B242" s="5" t="s">
+      <c r="B242" t="s">
         <v>829</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A243" s="5">
+      <c r="A243">
         <v>241</v>
       </c>
-      <c r="B243" s="5" t="s">
+      <c r="B243" t="s">
         <v>830</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A244" s="5">
+      <c r="A244">
         <v>242</v>
       </c>
-      <c r="B244" s="5" t="s">
+      <c r="B244" t="s">
         <v>831</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A245" s="5">
+        <v>243</v>
+      </c>
+      <c r="B245" s="5" t="s">
+        <v>897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 9210 - Set Arlington site to Inactive
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C39229
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3377" uniqueCount="899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3378" uniqueCount="900">
   <si>
     <t>SourceID</t>
   </si>
@@ -2743,6 +2743,9 @@
   </si>
   <si>
     <t>New sub-coaching reason to Attendance for CSR and Supervisor. Updated Dim SubCoaching Reason and Coaching Reason Selection tabs.</t>
+  </si>
+  <si>
+    <t>Set Arlington to Inactive in DIM Site table and WISO13 to 0 for all modules in Employee selection table</t>
   </si>
 </sst>
 </file>
@@ -3114,10 +3117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4177,6 +4180,23 @@
       </c>
       <c r="E63" t="s">
         <v>898</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>56</v>
+      </c>
+      <c r="B64" s="1">
+        <v>43073</v>
+      </c>
+      <c r="C64" t="s">
+        <v>432</v>
+      </c>
+      <c r="D64">
+        <v>9210</v>
+      </c>
+      <c r="E64" t="s">
+        <v>899</v>
       </c>
     </row>
   </sheetData>
@@ -31365,11 +31385,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -31379,7 +31397,7 @@
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -31392,8 +31410,11 @@
       <c r="D1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -31406,8 +31427,11 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -31420,8 +31444,11 @@
       <c r="D3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -31434,8 +31461,11 @@
       <c r="D4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -31448,8 +31478,11 @@
       <c r="D5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -31462,8 +31495,11 @@
       <c r="D6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -31476,8 +31512,11 @@
       <c r="D7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -31490,8 +31529,11 @@
       <c r="D8" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -31504,8 +31546,11 @@
       <c r="D9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -31518,8 +31563,11 @@
       <c r="D10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -31532,8 +31580,11 @@
       <c r="D11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -31546,8 +31597,11 @@
       <c r="D12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -31560,8 +31614,11 @@
       <c r="D13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -31574,8 +31631,11 @@
       <c r="D14" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -31588,8 +31648,11 @@
       <c r="D15" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -31602,8 +31665,11 @@
       <c r="D16" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -31616,8 +31682,11 @@
       <c r="D17" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -31630,8 +31699,11 @@
       <c r="D18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -31644,8 +31716,11 @@
       <c r="D19" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -31658,8 +31733,11 @@
       <c r="D20" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -31671,6 +31749,9 @@
       </c>
       <c r="D21" t="s">
         <v>81</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -34921,11 +35002,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -35075,13 +35154,13 @@
         <v>258</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -35317,29 +35396,6 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>325</v>
-      </c>
-      <c r="B18" t="s">
-        <v>326</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
         <v>1</v>
       </c>
     </row>

</xml_diff>